<commit_message>
Update a lot + change most class to static class + now can test system by using GET method + UI is under construction
</commit_message>
<xml_diff>
--- a/resource/led_stripe_html_template.xlsx
+++ b/resource/led_stripe_html_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snn2spade/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snn2spade/Project-Sourcecode/Arduino_project/LEDStripeController2/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="97">
   <si>
     <t>&lt;!DOCTYPE html&gt;</t>
   </si>
@@ -167,24 +167,6 @@
     <t>&lt;div class='list-group'&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='#' class='list-group-item active'&gt;Play Example&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Color Wipe&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Set Fire to the rain!&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Rainbow cycle&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Snow sparkle&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Twinkle&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;powered by snn2spade, 2017&lt;/p&gt;</t>
   </si>
   <si>
@@ -270,6 +252,72 @@
   </si>
   <si>
     <t>";</t>
+  </si>
+  <si>
+    <t>&lt;input id='modeInput' type='hidden' name='mode' value='-1'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='#' id="mode1" class='list-group-item list-group-item-action '&gt;Color Wipe&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='#' id="mode2" class='list-group-item list-group-item-action '&gt;Set Fire to the rain!&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='#' id="mode3" class='list-group-item list-group-item-action '&gt;Rainbow cycle&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='#' id="mode4" class='list-group-item list-group-item-action '&gt;Snow sparkle&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='#' id="mode5" class='list-group-item list-group-item-action '&gt;Twinkle&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>window.onload = function(){</t>
+  </si>
+  <si>
+    <t>let mode = $('#modeInput').val();</t>
+  </si>
+  <si>
+    <t>mode = parseInt(mode);</t>
+  </si>
+  <si>
+    <t>switch(mode){</t>
+  </si>
+  <si>
+    <t>case 1:</t>
+  </si>
+  <si>
+    <t>$('#mode1').addClass('active');</t>
+  </si>
+  <si>
+    <t>break;</t>
+  </si>
+  <si>
+    <t>case 2:</t>
+  </si>
+  <si>
+    <t>$('#mode2').addClass('active');</t>
+  </si>
+  <si>
+    <t>case 3:</t>
+  </si>
+  <si>
+    <t>$('#mode3').addClass('active');</t>
+  </si>
+  <si>
+    <t>case 4:</t>
+  </si>
+  <si>
+    <t>$('#mode4').addClass('active');</t>
+  </si>
+  <si>
+    <t>case 5:</t>
+  </si>
+  <si>
+    <t>$('#mode5').addClass('active');</t>
+  </si>
+  <si>
+    <t>};</t>
   </si>
 </sst>
 </file>
@@ -293,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,10 +374,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -604,24 +659,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="J125" sqref="J125"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>_xlfn.CONCAT(A1,B1,C1)</f>
@@ -630,13 +686,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(A2,B2,C2)</f>
@@ -645,13 +701,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -660,13 +716,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -675,13 +731,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -690,13 +746,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -705,13 +761,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -720,13 +776,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -735,13 +791,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -750,10 +806,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -762,13 +818,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -777,13 +833,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -792,13 +848,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -807,10 +863,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -819,13 +875,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -834,13 +890,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -849,13 +905,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -864,13 +920,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -879,13 +935,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -894,13 +950,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -909,13 +965,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -924,13 +980,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -939,13 +995,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -954,13 +1010,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -969,13 +1025,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -984,13 +1040,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -999,13 +1055,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1014,13 +1070,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1029,13 +1085,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1044,13 +1100,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1059,13 +1115,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1074,13 +1130,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1089,13 +1145,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1104,13 +1160,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1119,13 +1175,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1134,13 +1190,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D36" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1149,13 +1205,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D37" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1164,13 +1220,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D38" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1179,13 +1235,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D39" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1194,13 +1250,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D40" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1209,13 +1265,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D41" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1224,13 +1280,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D42" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1239,13 +1295,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D43" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1254,13 +1310,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D44" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1269,13 +1325,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D45" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1284,13 +1340,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1299,13 +1355,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B47" t="s">
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1314,13 +1370,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
         <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1329,13 +1385,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
         <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D49" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1344,13 +1400,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B50" t="s">
         <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D50" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1359,13 +1415,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D51" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1374,13 +1430,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D52" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1389,13 +1445,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D53" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1404,13 +1460,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D54" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1419,13 +1475,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
         <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D55" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1434,13 +1490,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D56" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1449,13 +1505,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D57" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1464,13 +1520,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D58" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1479,13 +1535,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D59" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1494,13 +1550,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D60" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1509,13 +1565,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D61" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1524,13 +1580,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
         <v>38</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D62" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1539,13 +1595,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B63" t="s">
         <v>39</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D63" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1554,13 +1610,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
         <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D64" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1569,13 +1625,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D65" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1584,13 +1640,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
         <v>41</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D66" s="2" t="str">
         <f t="shared" ref="D66:D129" si="1">_xlfn.CONCAT(A66,B66,C66)</f>
@@ -1599,13 +1655,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D67" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1614,13 +1670,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
         <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D68" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1629,13 +1685,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
         <v>26</v>
       </c>
       <c r="C69" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D69" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1644,13 +1700,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
         <v>42</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D70" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1659,13 +1715,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>28</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D71" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1674,13 +1730,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
         <v>43</v>
       </c>
       <c r="C72" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D72" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1689,13 +1745,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D73" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1704,13 +1760,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D74" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1719,13 +1775,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>37</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D75" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1734,13 +1790,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D76" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1749,13 +1805,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D77" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1764,13 +1820,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B78" t="s">
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D78" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1779,13 +1835,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B79" t="s">
         <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D79" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1794,13 +1850,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B80" t="s">
         <v>39</v>
       </c>
       <c r="C80" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D80" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1809,13 +1865,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
         <v>40</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D81" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1824,13 +1880,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D82" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1839,13 +1895,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
         <v>44</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D83" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1854,13 +1910,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
         <v>24</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D84" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1869,13 +1925,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D85" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1884,13 +1940,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B86" t="s">
         <v>45</v>
       </c>
       <c r="C86" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D86" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1899,103 +1955,103 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>79</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D87" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item active'&gt;Play Example&lt;/a&gt;";</v>
+        <v>res+="&lt;input id='modeInput' type='hidden' name='mode' value='-1'&gt;";</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D88" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Color Wipe&lt;/a&gt;";</v>
+        <v>res+="&lt;a href='#' id="mode1" class='list-group-item list-group-item-action '&gt;Color Wipe&lt;/a&gt;";</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C89" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D89" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Set Fire to the rain!&lt;/a&gt;";</v>
+        <v>res+="&lt;a href='#' id="mode2" class='list-group-item list-group-item-action '&gt;Set Fire to the rain!&lt;/a&gt;";</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C90" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D90" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Rainbow cycle&lt;/a&gt;";</v>
+        <v>res+="&lt;a href='#' id="mode3" class='list-group-item list-group-item-action '&gt;Rainbow cycle&lt;/a&gt;";</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>73</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C91" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D91" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Snow sparkle&lt;/a&gt;";</v>
+        <v>res+="&lt;a href='#' id="mode4" class='list-group-item list-group-item-action '&gt;Snow sparkle&lt;/a&gt;";</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C92" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D92" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>res+="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Twinkle&lt;/a&gt;";</v>
+        <v>res+="&lt;a href='#' id="mode5" class='list-group-item list-group-item-action '&gt;Twinkle&lt;/a&gt;";</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D93" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2004,13 +2060,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B94" t="s">
         <v>37</v>
       </c>
       <c r="C94" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D94" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2019,13 +2075,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B95" t="s">
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D95" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2034,13 +2090,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B96" t="s">
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D96" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2049,13 +2105,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B97" t="s">
         <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D97" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2064,13 +2120,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B98" t="s">
         <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D98" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2079,13 +2135,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B99" t="s">
         <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D99" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2094,13 +2150,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B100" t="s">
         <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D100" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2109,13 +2165,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
         <v>39</v>
       </c>
       <c r="C101" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D101" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2124,13 +2180,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
         <v>40</v>
       </c>
       <c r="C102" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D102" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2139,13 +2195,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B103" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C103" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D103" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2154,13 +2210,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B104" t="s">
         <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D104" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2169,13 +2225,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B105" t="s">
         <v>19</v>
       </c>
       <c r="C105" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D105" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2184,13 +2240,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B106" t="s">
         <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D106" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2199,13 +2255,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B107" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C107" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D107" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2214,13 +2270,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B108" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C108" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D108" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2229,13 +2285,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B109" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C109" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D109" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2244,13 +2300,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B110" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C110" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D110" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2259,13 +2315,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B111" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C111" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D111" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2274,13 +2330,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B112" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C112" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D112" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2289,13 +2345,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B113" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C113" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D113" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2304,13 +2360,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B114" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C114" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D114" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2319,13 +2375,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B115" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C115" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D115" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2334,13 +2390,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B116" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C116" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D116" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2349,13 +2405,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B117" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C117" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D117" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2364,13 +2420,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B118" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C118" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D118" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2379,13 +2435,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B119" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C119" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D119" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2394,13 +2450,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B120" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C120" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D120" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2409,13 +2465,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B121" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C121" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D121" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2424,13 +2480,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B122" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C122" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D122" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2439,13 +2495,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B123" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C123" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D123" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2454,13 +2510,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B124" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C124" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D124" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2469,13 +2525,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B125" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C125" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D125" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2484,13 +2540,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B126" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C126" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D126" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2499,13 +2555,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B127" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C127" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D127" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2514,13 +2570,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B128" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C128" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D128" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2529,13 +2585,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B129" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C129" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D129" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2544,28 +2600,28 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B130" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C130" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D130" s="2" t="str">
-        <f t="shared" ref="D130:D168" si="2">_xlfn.CONCAT(A130,B130,C130)</f>
+        <f t="shared" ref="D130:D162" si="2">_xlfn.CONCAT(A130,B130,C130)</f>
         <v>res+="//alert('Send completed.');";</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B131" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C131" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D131" s="2" t="str">
         <f t="shared" si="2"/>
@@ -2574,347 +2630,512 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B132" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C132" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D132" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="&lt;/script&gt;";</v>
+        <v>res+="window.onload = function(){";</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B133" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C133" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D133" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="&lt;/body&gt;";</v>
+        <v>res+="let mode = $('#modeInput').val();";</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B134" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C134" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D134" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="&lt;/html&gt;";</v>
+        <v>res+="mode = parseInt(mode);";</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B135" t="s">
+        <v>84</v>
       </c>
       <c r="C135" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D135" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="switch(mode){";</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B136" t="s">
+        <v>85</v>
       </c>
       <c r="C136" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D136" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="case 1:";</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B137" t="s">
+        <v>86</v>
       </c>
       <c r="C137" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D137" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="$('#mode1').addClass('active');";</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B138" t="s">
+        <v>87</v>
       </c>
       <c r="C138" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D138" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="break;";</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B139" t="s">
+        <v>88</v>
       </c>
       <c r="C139" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D139" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="case 2:";</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B140" t="s">
+        <v>89</v>
       </c>
       <c r="C140" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D140" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="$('#mode2').addClass('active');";</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B141" t="s">
+        <v>87</v>
       </c>
       <c r="C141" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D141" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="break;";</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B142" t="s">
+        <v>90</v>
       </c>
       <c r="C142" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D142" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="case 3:";</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B143" t="s">
+        <v>91</v>
       </c>
       <c r="C143" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D143" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="$('#mode3').addClass('active');";</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B144" t="s">
+        <v>87</v>
       </c>
       <c r="C144" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D144" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="break;";</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B145" t="s">
+        <v>92</v>
       </c>
       <c r="C145" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D145" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="case 4:";</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B146" t="s">
+        <v>93</v>
       </c>
       <c r="C146" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D146" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="$('#mode4').addClass('active');";</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B147" t="s">
+        <v>87</v>
       </c>
       <c r="C147" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D147" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="break;";</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B148" t="s">
+        <v>94</v>
       </c>
       <c r="C148" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D148" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="case 5:";</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B149" t="s">
+        <v>95</v>
       </c>
       <c r="C149" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D149" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="$('#mode5').addClass('active');";</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B150" t="s">
+        <v>87</v>
       </c>
       <c r="C150" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D150" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>res+="";</v>
+        <v>res+="break;";</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>73</v>
+      </c>
+      <c r="B151" t="s">
+        <v>50</v>
+      </c>
+      <c r="C151" t="s">
+        <v>74</v>
+      </c>
       <c r="D151" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="}";</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>73</v>
+      </c>
+      <c r="B152" t="s">
+        <v>96</v>
+      </c>
+      <c r="C152" t="s">
+        <v>74</v>
+      </c>
       <c r="D152" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="};";</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>73</v>
+      </c>
+      <c r="B153" t="s">
+        <v>70</v>
+      </c>
+      <c r="C153" t="s">
+        <v>74</v>
+      </c>
       <c r="D153" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="&lt;/script&gt;";</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>73</v>
+      </c>
+      <c r="B154" t="s">
+        <v>71</v>
+      </c>
+      <c r="C154" t="s">
+        <v>74</v>
+      </c>
       <c r="D154" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="&lt;/body&gt;";</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>73</v>
+      </c>
+      <c r="B155" t="s">
+        <v>72</v>
+      </c>
+      <c r="C155" t="s">
+        <v>74</v>
+      </c>
       <c r="D155" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="&lt;/html&gt;";</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>73</v>
+      </c>
+      <c r="C156" t="s">
+        <v>74</v>
+      </c>
       <c r="D156" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="";</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>73</v>
+      </c>
+      <c r="C157" t="s">
+        <v>74</v>
+      </c>
       <c r="D157" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="";</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>73</v>
+      </c>
+      <c r="C158" t="s">
+        <v>74</v>
+      </c>
       <c r="D158" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="";</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>73</v>
+      </c>
+      <c r="C159" t="s">
+        <v>74</v>
+      </c>
       <c r="D159" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>res+="";</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>73</v>
+      </c>
+      <c r="C160" t="s">
+        <v>74</v>
+      </c>
       <c r="D160" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+        <v>res+="";</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>73</v>
+      </c>
+      <c r="C161" t="s">
+        <v>74</v>
+      </c>
       <c r="D161" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+        <v>res+="";</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>73</v>
+      </c>
+      <c r="C162" t="s">
+        <v>74</v>
+      </c>
       <c r="D162" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D163" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D164" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D165" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D166" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D167" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D168" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>res+="";</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>73</v>
+      </c>
+      <c r="C163" t="s">
+        <v>74</v>
+      </c>
+      <c r="D163" s="2" t="e">
+        <f>_xlfn.CONCAT(A163,#REF!,B163)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>73</v>
+      </c>
+      <c r="C164" t="s">
+        <v>74</v>
+      </c>
+      <c r="D164" s="2" t="e">
+        <f>_xlfn.CONCAT(A164,#REF!,B164)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>73</v>
+      </c>
+      <c r="C165" t="s">
+        <v>74</v>
+      </c>
+      <c r="D165" s="2" t="e">
+        <f>_xlfn.CONCAT(A165,#REF!,B165)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>73</v>
+      </c>
+      <c r="C166" t="s">
+        <v>74</v>
+      </c>
+      <c r="D166" s="2" t="e">
+        <f>_xlfn.CONCAT(A166,#REF!,B166)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D167" s="3" t="e">
+        <f>_xlfn.CONCAT(A167,#REF!,B167)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D168" s="2" t="e">
+        <f>_xlfn.CONCAT(A168,#REF!,B168)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -2925,12 +3146,11 @@
     <hyperlink ref="B9" r:id="rId4"/>
     <hyperlink ref="B11" r:id="rId5"/>
     <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B87" display="&lt;a href='#' class='list-group-item active'&gt;Play Example&lt;/a&gt;"/>
-    <hyperlink ref="B88" display="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Color Wipe&lt;/a&gt;"/>
-    <hyperlink ref="B89" display="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Set Fire to the rain!&lt;/a&gt;"/>
-    <hyperlink ref="B90" display="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Rainbow cycle&lt;/a&gt;"/>
-    <hyperlink ref="B91" display="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Snow sparkle&lt;/a&gt;"/>
-    <hyperlink ref="B92" display="&lt;a href='#' class='list-group-item list-group-item-action disabled'&gt;Twinkle&lt;/a&gt;"/>
+    <hyperlink ref="B88" display="&lt;a href='#' id=&quot;mode1&quot; class='list-group-item list-group-item-action '&gt;Color Wipe&lt;/a&gt;"/>
+    <hyperlink ref="B89" display="&lt;a href='#' id=&quot;mode2&quot; class='list-group-item list-group-item-action '&gt;Set Fire to the rain!&lt;/a&gt;"/>
+    <hyperlink ref="B90" display="&lt;a href='#' id=&quot;mode3&quot; class='list-group-item list-group-item-action '&gt;Rainbow cycle&lt;/a&gt;"/>
+    <hyperlink ref="B91" display="&lt;a href='#' id=&quot;mode4&quot; class='list-group-item list-group-item-action '&gt;Snow sparkle&lt;/a&gt;"/>
+    <hyperlink ref="B92" display="&lt;a href='#' id=&quot;mode5&quot; class='list-group-item list-group-item-action '&gt;Twinkle&lt;/a&gt;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>